<commit_message>
add new LCS exercise
</commit_message>
<xml_diff>
--- a/lcs.xlsx
+++ b/lcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\rocco\uni\algorithms-and-data-structures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocco\uni\algorithms-and-data-structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89C6CF1-BAFF-488B-8362-4ACE31C4810F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1A01B1-C021-4AAB-B172-A587DC5800D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="2355" windowWidth="38040" windowHeight="18525" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AGGTAB – GXTXAYB" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="albero – tabella" sheetId="4" r:id="rId4"/>
     <sheet name="programmazione – informatica" sheetId="5" r:id="rId5"/>
     <sheet name="heap – pea" sheetId="6" r:id="rId6"/>
+    <sheet name="XMJYAUZ – MZJAWXU" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="41">
   <si>
     <t>epsilon</t>
   </si>
@@ -145,6 +146,22 @@
   </si>
   <si>
     <t>LCS = EA</t>
+  </si>
+  <si>
+    <t>X = XMJYAUZ
+Y = MZJAWXU</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>LCS = MJAZ</t>
   </si>
 </sst>
 </file>
@@ -229,7 +246,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -758,11 +775,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -962,6 +994,18 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -971,35 +1015,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1341,28 +1385,28 @@
     </row>
     <row r="8" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
     </row>
     <row r="9" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
     </row>
     <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
@@ -1676,26 +1720,26 @@
     </row>
     <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
     </row>
     <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
@@ -2010,30 +2054,30 @@
     </row>
     <row r="8" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
     </row>
     <row r="9" spans="1:11" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="71"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="39"/>
@@ -2340,28 +2384,28 @@
     </row>
     <row r="8" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
     </row>
     <row r="9" spans="1:11" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="39"/>
@@ -2675,42 +2719,42 @@
     </row>
     <row r="8" spans="1:18" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67"/>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-      <c r="M8" s="67"/>
-      <c r="N8" s="67"/>
-      <c r="O8" s="67"/>
-      <c r="P8" s="67"/>
-      <c r="Q8" s="67"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="71"/>
+      <c r="P8" s="71"/>
+      <c r="Q8" s="71"/>
     </row>
     <row r="9" spans="1:18" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="71"/>
+      <c r="N9" s="71"/>
+      <c r="O9" s="71"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
     </row>
     <row r="10" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="39"/>
@@ -3402,8 +3446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944E67B5-D24B-4D57-B773-53A1A9F90F92}">
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3452,20 +3496,20 @@
     </row>
     <row r="8" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
     </row>
     <row r="9" spans="1:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
@@ -3486,13 +3530,13 @@
       <c r="B11" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="75">
-        <v>0</v>
-      </c>
-      <c r="D11" s="74">
-        <v>0</v>
-      </c>
-      <c r="E11" s="76">
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="68">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16">
         <v>0</v>
       </c>
       <c r="F11" s="33">
@@ -3503,13 +3547,13 @@
       <c r="B12" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="77">
+      <c r="C12" s="7">
         <v>0</v>
       </c>
       <c r="D12" s="22">
         <v>0</v>
       </c>
-      <c r="E12" s="73">
+      <c r="E12" s="2">
         <v>0</v>
       </c>
       <c r="F12" s="4">
@@ -3520,10 +3564,10 @@
       <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="77">
-        <v>0</v>
-      </c>
-      <c r="D13" s="73">
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
         <v>0</v>
       </c>
       <c r="E13" s="20">
@@ -3537,16 +3581,16 @@
       <c r="B14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="77">
-        <v>0</v>
-      </c>
-      <c r="D14" s="73">
-        <v>0</v>
-      </c>
-      <c r="E14" s="73">
-        <v>1</v>
-      </c>
-      <c r="F14" s="72">
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="67">
         <v>2</v>
       </c>
     </row>
@@ -3554,13 +3598,13 @@
       <c r="B15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="78">
-        <v>0</v>
-      </c>
-      <c r="D15" s="79">
-        <v>1</v>
-      </c>
-      <c r="E15" s="79">
+      <c r="C15" s="69">
+        <v>0</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
         <v>1</v>
       </c>
       <c r="F15" s="66">
@@ -3583,4 +3627,370 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B8371F-EBF9-4D6D-98D1-0AD663E0C154}">
+  <dimension ref="A2:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.7109375" style="1" customWidth="1"/>
+    <col min="2" max="12" width="20.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="40.7109375" style="1" customWidth="1"/>
+    <col min="14" max="16" width="20.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="82" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="83" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+    </row>
+    <row r="9" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="73"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+    </row>
+    <row r="10" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15"/>
+      <c r="C10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="75">
+        <v>0</v>
+      </c>
+      <c r="E12" s="20">
+        <v>1</v>
+      </c>
+      <c r="F12" s="75">
+        <v>1</v>
+      </c>
+      <c r="G12" s="75">
+        <v>1</v>
+      </c>
+      <c r="H12" s="75">
+        <v>1</v>
+      </c>
+      <c r="I12" s="75">
+        <v>1</v>
+      </c>
+      <c r="J12" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="75">
+        <v>0</v>
+      </c>
+      <c r="E13" s="22">
+        <v>1</v>
+      </c>
+      <c r="F13" s="75">
+        <v>1</v>
+      </c>
+      <c r="G13" s="75">
+        <v>1</v>
+      </c>
+      <c r="H13" s="75">
+        <v>1</v>
+      </c>
+      <c r="I13" s="75">
+        <v>1</v>
+      </c>
+      <c r="J13" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="75">
+        <v>0</v>
+      </c>
+      <c r="E14" s="75">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20">
+        <v>2</v>
+      </c>
+      <c r="G14" s="22">
+        <v>2</v>
+      </c>
+      <c r="H14" s="75">
+        <v>2</v>
+      </c>
+      <c r="I14" s="75">
+        <v>2</v>
+      </c>
+      <c r="J14" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="75">
+        <v>0</v>
+      </c>
+      <c r="E15" s="75">
+        <v>1</v>
+      </c>
+      <c r="F15" s="75">
+        <v>2</v>
+      </c>
+      <c r="G15" s="75">
+        <v>2</v>
+      </c>
+      <c r="H15" s="20">
+        <v>3</v>
+      </c>
+      <c r="I15" s="75">
+        <v>3</v>
+      </c>
+      <c r="J15" s="76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="75">
+        <v>0</v>
+      </c>
+      <c r="E16" s="75">
+        <v>1</v>
+      </c>
+      <c r="F16" s="75">
+        <v>2</v>
+      </c>
+      <c r="G16" s="75">
+        <v>2</v>
+      </c>
+      <c r="H16" s="22">
+        <v>3</v>
+      </c>
+      <c r="I16" s="77">
+        <v>3</v>
+      </c>
+      <c r="J16" s="76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="80">
+        <v>0</v>
+      </c>
+      <c r="D17" s="75">
+        <v>1</v>
+      </c>
+      <c r="E17" s="75">
+        <v>1</v>
+      </c>
+      <c r="F17" s="75">
+        <v>2</v>
+      </c>
+      <c r="G17" s="75">
+        <v>2</v>
+      </c>
+      <c r="H17" s="22">
+        <v>3</v>
+      </c>
+      <c r="I17" s="75">
+        <v>3</v>
+      </c>
+      <c r="J17" s="76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="78">
+        <v>1</v>
+      </c>
+      <c r="E18" s="78">
+        <v>1</v>
+      </c>
+      <c r="F18" s="78">
+        <v>2</v>
+      </c>
+      <c r="G18" s="78">
+        <v>2</v>
+      </c>
+      <c r="H18" s="78">
+        <v>3</v>
+      </c>
+      <c r="I18" s="81">
+        <v>4</v>
+      </c>
+      <c r="J18" s="79">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="21" x14ac:dyDescent="0.25">
+      <c r="B21" s="70" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="70"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B8:J9"/>
+    <mergeCell ref="B21:J21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>